<commit_message>
work done 24th April
</commit_message>
<xml_diff>
--- a/experimental_results.xlsx
+++ b/experimental_results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="32">
   <si>
     <t>Dataset</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>intermediate</t>
+  </si>
+  <si>
+    <t>lambda s</t>
+  </si>
+  <si>
+    <t>Coarse Search</t>
+  </si>
+  <si>
+    <t>RMSE u</t>
+  </si>
+  <si>
+    <t>RMSE v</t>
+  </si>
+  <si>
+    <t>lambda t</t>
   </si>
 </sst>
 </file>
@@ -257,77 +272,85 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -407,10 +430,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:N30"/>
+  <dimension ref="B1:V43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P24" activeCellId="0" sqref="P24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T28" activeCellId="0" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -420,9 +443,9 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.1020408163265"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.9948979591837"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.3316326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.780612244898"/>
     <col collapsed="false" hidden="false" max="11" min="8" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.0765306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.8061224489796"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -484,7 +507,7 @@
       </c>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -500,7 +523,7 @@
       <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -515,7 +538,7 @@
       <c r="K5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -547,7 +570,7 @@
       <c r="H6" s="1" t="n">
         <v>-96.495768</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="4" t="n">
         <v>93.935238</v>
       </c>
       <c r="J6" s="1" t="n">
@@ -576,12 +599,12 @@
       <c r="F7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="0"/>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
-      <c r="J7" s="0"/>
-      <c r="K7" s="0"/>
-      <c r="L7" s="0"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="n">
@@ -654,76 +677,76 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="n">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6" t="n">
         <v>-21.321</v>
       </c>
-      <c r="I11" s="4" t="n">
+      <c r="I11" s="6" t="n">
         <v>6.261</v>
       </c>
-      <c r="J11" s="4" t="n">
+      <c r="J11" s="6" t="n">
         <v>-0.872</v>
       </c>
-      <c r="K11" s="4" t="n">
+      <c r="K11" s="6" t="n">
         <v>8.512</v>
       </c>
-      <c r="L11" s="4" t="n">
+      <c r="L11" s="6" t="n">
         <v>22.1894</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="7" t="n">
+      <c r="D13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="9" t="n">
         <v>0.1</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="7" t="n">
+      <c r="F13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="9" t="n">
         <v>20274</v>
       </c>
-      <c r="H13" s="7" t="n">
+      <c r="H13" s="9" t="n">
         <v>-92.178968</v>
       </c>
-      <c r="I13" s="7" t="n">
+      <c r="I13" s="9" t="n">
         <v>88.699041</v>
       </c>
-      <c r="J13" s="7" t="n">
+      <c r="J13" s="9" t="n">
         <v>-107.951246</v>
       </c>
-      <c r="K13" s="7" t="n">
+      <c r="K13" s="9" t="n">
         <v>89.767693</v>
       </c>
-      <c r="L13" s="7" t="n">
+      <c r="L13" s="9" t="n">
         <v>109.011066</v>
       </c>
-      <c r="M13" s="7" t="n">
+      <c r="M13" s="9" t="n">
         <v>11.1759</v>
       </c>
-      <c r="N13" s="8" t="n">
+      <c r="N13" s="10" t="n">
         <v>4.6497</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="5"/>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -756,13 +779,13 @@
       <c r="M14" s="1" t="n">
         <v>10.884</v>
       </c>
-      <c r="N14" s="10" t="n">
+      <c r="N14" s="12" t="n">
         <v>3.8964</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5"/>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -792,94 +815,94 @@
       <c r="L15" s="1" t="n">
         <v>15.214065</v>
       </c>
-      <c r="M15" s="11" t="n">
+      <c r="M15" s="13" t="n">
         <v>10.8489</v>
       </c>
-      <c r="N15" s="12" t="n">
+      <c r="N15" s="14" t="n">
         <v>3.714</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="14" t="n">
+      <c r="D16" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="16" t="n">
         <v>100</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="14" t="n">
+      <c r="F16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="16" t="n">
         <v>397</v>
       </c>
-      <c r="H16" s="14" t="n">
+      <c r="H16" s="16" t="n">
         <v>-4.051817</v>
       </c>
-      <c r="I16" s="14" t="n">
+      <c r="I16" s="16" t="n">
         <v>4.039457</v>
       </c>
-      <c r="J16" s="14" t="n">
+      <c r="J16" s="16" t="n">
         <v>-4.460545</v>
       </c>
-      <c r="K16" s="14" t="n">
+      <c r="K16" s="16" t="n">
         <v>3.946301</v>
       </c>
-      <c r="L16" s="14" t="n">
+      <c r="L16" s="16" t="n">
         <v>4.980264</v>
       </c>
-      <c r="M16" s="14" t="n">
+      <c r="M16" s="16" t="n">
         <v>10.9113</v>
       </c>
-      <c r="N16" s="15" t="n">
+      <c r="N16" s="17" t="n">
         <v>3.747</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5"/>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="7" t="n">
+      <c r="D17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="9" t="n">
         <v>0.1</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="7" t="n">
+      <c r="F17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="9" t="n">
         <v>17453</v>
       </c>
-      <c r="H17" s="7" t="n">
+      <c r="H17" s="9" t="n">
         <v>-47.500071</v>
       </c>
-      <c r="I17" s="7" t="n">
+      <c r="I17" s="9" t="n">
         <v>47.730562</v>
       </c>
-      <c r="J17" s="7" t="n">
+      <c r="J17" s="9" t="n">
         <v>-45.098676</v>
       </c>
-      <c r="K17" s="7" t="n">
+      <c r="K17" s="9" t="n">
         <v>43.035501</v>
       </c>
-      <c r="L17" s="7" t="n">
+      <c r="L17" s="9" t="n">
         <v>49.112178</v>
       </c>
-      <c r="M17" s="7" t="n">
+      <c r="M17" s="9" t="n">
         <v>10.9466</v>
       </c>
-      <c r="N17" s="8" t="n">
+      <c r="N17" s="10" t="n">
         <v>4.5271</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5"/>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="7"/>
+      <c r="C18" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -891,34 +914,34 @@
       <c r="F18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="5" t="n">
+      <c r="G18" s="7" t="n">
         <v>7439</v>
       </c>
-      <c r="H18" s="5" t="n">
+      <c r="H18" s="7" t="n">
         <v>-24.908582</v>
       </c>
-      <c r="I18" s="5" t="n">
+      <c r="I18" s="7" t="n">
         <v>24.308736</v>
       </c>
-      <c r="J18" s="5" t="n">
+      <c r="J18" s="7" t="n">
         <v>-24.919485</v>
       </c>
-      <c r="K18" s="5" t="n">
+      <c r="K18" s="7" t="n">
         <v>24.345496</v>
       </c>
-      <c r="L18" s="5" t="n">
+      <c r="L18" s="7" t="n">
         <v>26.411453</v>
       </c>
-      <c r="M18" s="5" t="n">
+      <c r="M18" s="7" t="n">
         <v>10.7514</v>
       </c>
-      <c r="N18" s="10" t="n">
+      <c r="N18" s="12" t="n">
         <v>4.0257</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="C19" s="9" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -930,34 +953,34 @@
       <c r="F19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="5" t="n">
+      <c r="G19" s="7" t="n">
         <v>6104</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="H19" s="7" t="n">
         <v>-21.335275</v>
       </c>
-      <c r="I19" s="5" t="n">
+      <c r="I19" s="7" t="n">
         <v>19.376467</v>
       </c>
-      <c r="J19" s="5" t="n">
+      <c r="J19" s="7" t="n">
         <v>-21.177473</v>
       </c>
-      <c r="K19" s="5" t="n">
+      <c r="K19" s="7" t="n">
         <v>20.7185</v>
       </c>
-      <c r="L19" s="5" t="n">
+      <c r="L19" s="7" t="n">
         <v>21.863183</v>
       </c>
-      <c r="M19" s="5" t="n">
+      <c r="M19" s="7" t="n">
         <v>10.7216</v>
       </c>
-      <c r="N19" s="10" t="n">
+      <c r="N19" s="12" t="n">
         <v>3.9248</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5"/>
-      <c r="C20" s="9" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -987,190 +1010,212 @@
       <c r="L20" s="1" t="n">
         <v>20.299499</v>
       </c>
-      <c r="M20" s="11" t="n">
+      <c r="M20" s="18" t="n">
         <v>10.711</v>
       </c>
-      <c r="N20" s="10" t="n">
+      <c r="N20" s="12" t="n">
         <v>3.8831</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="5"/>
-      <c r="C21" s="9" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>4705</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>-17.857336</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>15.978126</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>-17.188612</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>16.521024</v>
+      </c>
+      <c r="L21" s="1" t="n">
+        <v>17.973561</v>
+      </c>
+      <c r="M21" s="18" t="n">
+        <v>10.7004</v>
+      </c>
+      <c r="N21" s="12" t="n">
+        <v>3.8183</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="7"/>
+      <c r="C22" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>4117</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>-16.124641</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>14.64901</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <v>-15.714903</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <v>14.633416</v>
+      </c>
+      <c r="L22" s="1" t="n">
+        <v>16.274808</v>
+      </c>
+      <c r="M22" s="13" t="n">
+        <v>10.6983</v>
+      </c>
+      <c r="N22" s="12" t="n">
+        <v>3.7805</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="7"/>
+      <c r="C23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="16"/>
-      <c r="N21" s="10"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="5"/>
-      <c r="C22" s="9" t="s">
+      <c r="F23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>3684</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>-14.768498</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>13.532942</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <v>-14.553587</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>13.267442</v>
+      </c>
+      <c r="L23" s="1" t="n">
+        <v>15.189129</v>
+      </c>
+      <c r="M23" s="18" t="n">
+        <v>10.6995</v>
+      </c>
+      <c r="N23" s="12" t="n">
+        <v>3.7558</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="7"/>
+      <c r="C24" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="1" t="n">
+      <c r="D24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>3342</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>-13.669898</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>12.581091</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <v>-13.770426</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>12.473041</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <v>14.274543</v>
+      </c>
+      <c r="M24" s="18" t="n">
+        <v>10.7024</v>
+      </c>
+      <c r="N24" s="12" t="n">
+        <v>3.7385</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="7"/>
+      <c r="C25" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="1" t="n">
+      <c r="F25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="1" t="n">
         <v>2498</v>
       </c>
-      <c r="H22" s="1" t="n">
+      <c r="H25" s="1" t="n">
         <v>-10.941038</v>
       </c>
-      <c r="I22" s="1" t="n">
+      <c r="I25" s="1" t="n">
         <v>9.845384</v>
       </c>
-      <c r="J22" s="1" t="n">
+      <c r="J25" s="1" t="n">
         <v>-11.874378</v>
       </c>
-      <c r="K22" s="1" t="n">
+      <c r="K25" s="1" t="n">
         <v>10.200604</v>
       </c>
-      <c r="L22" s="1" t="n">
+      <c r="L25" s="1" t="n">
         <v>11.939979</v>
       </c>
-      <c r="M22" s="16" t="n">
+      <c r="M25" s="18" t="n">
         <v>10.7165</v>
       </c>
-      <c r="N22" s="10" t="n">
+      <c r="N25" s="12" t="n">
         <v>3.7023</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="5"/>
-      <c r="C23" s="9" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="7"/>
+      <c r="C26" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>1624</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <v>-8.054333</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <v>7.204148</v>
-      </c>
-      <c r="J23" s="1" t="n">
-        <v>-9.004037</v>
-      </c>
-      <c r="K23" s="1" t="n">
-        <v>7.73715</v>
-      </c>
-      <c r="L23" s="1" t="n">
-        <v>9.057529</v>
-      </c>
-      <c r="M23" s="1" t="n">
-        <v>10.7461</v>
-      </c>
-      <c r="N23" s="12" t="n">
-        <v>3.6767</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="5"/>
-      <c r="C24" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="14" t="n">
-        <v>100</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="14" t="n">
-        <v>424</v>
-      </c>
-      <c r="H24" s="14" t="n">
-        <v>-2.645342</v>
-      </c>
-      <c r="I24" s="14" t="n">
-        <v>2.518114</v>
-      </c>
-      <c r="J24" s="14" t="n">
-        <v>-2.519984</v>
-      </c>
-      <c r="K24" s="14" t="n">
-        <v>3.48677</v>
-      </c>
-      <c r="L24" s="14" t="n">
-        <v>3.487102</v>
-      </c>
-      <c r="M24" s="14" t="n">
-        <v>10.8708</v>
-      </c>
-      <c r="N24" s="15" t="n">
-        <v>3.7085</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="5"/>
-      <c r="C25" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="7" t="n">
-        <v>5676</v>
-      </c>
-      <c r="H25" s="7" t="n">
-        <v>-20.549665</v>
-      </c>
-      <c r="I25" s="7" t="n">
-        <v>20.363776</v>
-      </c>
-      <c r="J25" s="7" t="n">
-        <v>-20.232003</v>
-      </c>
-      <c r="K25" s="7" t="n">
-        <v>19.518608</v>
-      </c>
-      <c r="L25" s="7" t="n">
-        <v>20.843222</v>
-      </c>
-      <c r="M25" s="7" t="n">
-        <v>10.7437</v>
-      </c>
-      <c r="N25" s="8" t="n">
-        <v>3.903</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="5"/>
-      <c r="C26" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>23</v>
@@ -1182,112 +1227,112 @@
         <v>19</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>1560</v>
+        <v>1624</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>-8.323227</v>
+        <v>-8.054333</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>7.194654</v>
+        <v>7.204148</v>
       </c>
       <c r="J26" s="1" t="n">
-        <v>-8.862994</v>
+        <v>-9.004037</v>
       </c>
       <c r="K26" s="1" t="n">
-        <v>8.173916</v>
+        <v>7.73715</v>
       </c>
       <c r="L26" s="1" t="n">
-        <v>8.914189</v>
-      </c>
-      <c r="M26" s="11" t="n">
-        <v>10.7434</v>
-      </c>
-      <c r="N26" s="12" t="n">
-        <v>3.6933</v>
+        <v>9.057529</v>
+      </c>
+      <c r="M26" s="1" t="n">
+        <v>10.7461</v>
+      </c>
+      <c r="N26" s="14" t="n">
+        <v>3.6767</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="5"/>
-      <c r="C27" s="13" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="16" t="n">
+        <v>100</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="16" t="n">
+        <v>424</v>
+      </c>
+      <c r="H27" s="16" t="n">
+        <v>-2.645342</v>
+      </c>
+      <c r="I27" s="16" t="n">
+        <v>2.518114</v>
+      </c>
+      <c r="J27" s="16" t="n">
+        <v>-2.519984</v>
+      </c>
+      <c r="K27" s="16" t="n">
+        <v>3.48677</v>
+      </c>
+      <c r="L27" s="16" t="n">
+        <v>3.487102</v>
+      </c>
+      <c r="M27" s="16" t="n">
+        <v>10.8708</v>
+      </c>
+      <c r="N27" s="17" t="n">
+        <v>3.7085</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="7"/>
+      <c r="C28" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="14" t="n">
-        <v>100</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="14" t="n">
-        <v>422</v>
-      </c>
-      <c r="H27" s="14" t="n">
-        <v>-2.739102</v>
-      </c>
-      <c r="I27" s="14" t="n">
-        <v>2.57844</v>
-      </c>
-      <c r="J27" s="14" t="n">
-        <v>-2.532031</v>
-      </c>
-      <c r="K27" s="14" t="n">
-        <v>3.572645</v>
-      </c>
-      <c r="L27" s="14" t="n">
-        <v>3.595007</v>
-      </c>
-      <c r="M27" s="14" t="n">
-        <v>10.8665</v>
-      </c>
-      <c r="N27" s="15" t="n">
-        <v>3.7138</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="5"/>
-      <c r="C28" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="7" t="n">
+      <c r="D28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="7" t="n">
-        <v>7166</v>
-      </c>
-      <c r="H28" s="7" t="n">
-        <v>-36.461799</v>
-      </c>
-      <c r="I28" s="7" t="n">
-        <v>34.906583</v>
-      </c>
-      <c r="J28" s="7" t="n">
-        <v>-32.986626</v>
-      </c>
-      <c r="K28" s="7" t="n">
-        <v>34.218116</v>
-      </c>
-      <c r="L28" s="7" t="n">
-        <v>39.988652</v>
-      </c>
-      <c r="M28" s="7" t="n">
-        <v>10.9154</v>
-      </c>
-      <c r="N28" s="8" t="n">
-        <v>4.442</v>
+      <c r="F28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="9" t="n">
+        <v>5676</v>
+      </c>
+      <c r="H28" s="9" t="n">
+        <v>-20.549665</v>
+      </c>
+      <c r="I28" s="9" t="n">
+        <v>20.363776</v>
+      </c>
+      <c r="J28" s="9" t="n">
+        <v>-20.232003</v>
+      </c>
+      <c r="K28" s="9" t="n">
+        <v>19.518608</v>
+      </c>
+      <c r="L28" s="9" t="n">
+        <v>20.843222</v>
+      </c>
+      <c r="M28" s="9" t="n">
+        <v>10.7437</v>
+      </c>
+      <c r="N28" s="10" t="n">
+        <v>3.903</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="5"/>
-      <c r="C29" s="9" t="s">
-        <v>26</v>
+      <c r="B29" s="7"/>
+      <c r="C29" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>23</v>
@@ -1299,73 +1344,432 @@
         <v>19</v>
       </c>
       <c r="G29" s="1" t="n">
+        <v>1560</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>-8.323227</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>7.194654</v>
+      </c>
+      <c r="J29" s="1" t="n">
+        <v>-8.862994</v>
+      </c>
+      <c r="K29" s="1" t="n">
+        <v>8.173916</v>
+      </c>
+      <c r="L29" s="1" t="n">
+        <v>8.914189</v>
+      </c>
+      <c r="M29" s="13" t="n">
+        <v>10.7434</v>
+      </c>
+      <c r="N29" s="14" t="n">
+        <v>3.6933</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="7"/>
+      <c r="C30" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="16" t="n">
+        <v>100</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="16" t="n">
+        <v>422</v>
+      </c>
+      <c r="H30" s="16" t="n">
+        <v>-2.739102</v>
+      </c>
+      <c r="I30" s="16" t="n">
+        <v>2.57844</v>
+      </c>
+      <c r="J30" s="16" t="n">
+        <v>-2.532031</v>
+      </c>
+      <c r="K30" s="16" t="n">
+        <v>3.572645</v>
+      </c>
+      <c r="L30" s="16" t="n">
+        <v>3.595007</v>
+      </c>
+      <c r="M30" s="16" t="n">
+        <v>10.8665</v>
+      </c>
+      <c r="N30" s="17" t="n">
+        <v>3.7138</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="7"/>
+      <c r="C31" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="9" t="n">
+        <v>7166</v>
+      </c>
+      <c r="H31" s="9" t="n">
+        <v>-36.461799</v>
+      </c>
+      <c r="I31" s="9" t="n">
+        <v>34.906583</v>
+      </c>
+      <c r="J31" s="9" t="n">
+        <v>-32.986626</v>
+      </c>
+      <c r="K31" s="9" t="n">
+        <v>34.218116</v>
+      </c>
+      <c r="L31" s="9" t="n">
+        <v>39.988652</v>
+      </c>
+      <c r="M31" s="9" t="n">
+        <v>10.9154</v>
+      </c>
+      <c r="N31" s="10" t="n">
+        <v>4.442</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="7"/>
+      <c r="C32" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="1" t="n">
         <v>2152</v>
       </c>
-      <c r="H29" s="1" t="n">
+      <c r="H32" s="1" t="n">
         <v>-13.389012</v>
       </c>
-      <c r="I29" s="1" t="n">
+      <c r="I32" s="1" t="n">
         <v>13.598849</v>
       </c>
-      <c r="J29" s="1" t="n">
+      <c r="J32" s="1" t="n">
         <v>-12.976157</v>
       </c>
-      <c r="K29" s="1" t="n">
+      <c r="K32" s="1" t="n">
         <v>13.6188</v>
       </c>
-      <c r="L29" s="1" t="n">
+      <c r="L32" s="1" t="n">
         <v>15.751995</v>
       </c>
-      <c r="M29" s="11" t="n">
+      <c r="M32" s="13" t="n">
         <v>10.7621</v>
       </c>
-      <c r="N29" s="10" t="n">
+      <c r="N32" s="12" t="n">
         <v>4.0752</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="5"/>
-      <c r="C30" s="13" t="s">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="7"/>
+      <c r="C33" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="14" t="n">
+      <c r="D33" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="16" t="n">
         <v>100</v>
       </c>
-      <c r="F30" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="14" t="n">
+      <c r="F33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="16" t="n">
         <v>609</v>
       </c>
-      <c r="H30" s="14" t="n">
+      <c r="H33" s="16" t="n">
         <v>-4.777272</v>
       </c>
-      <c r="I30" s="14" t="n">
+      <c r="I33" s="16" t="n">
         <v>4.41054</v>
       </c>
-      <c r="J30" s="14" t="n">
+      <c r="J33" s="16" t="n">
         <v>-4.920523</v>
       </c>
-      <c r="K30" s="14" t="n">
+      <c r="K33" s="16" t="n">
         <v>3.767666</v>
       </c>
-      <c r="L30" s="14" t="n">
+      <c r="L33" s="16" t="n">
         <v>4.942139</v>
       </c>
-      <c r="M30" s="14" t="n">
+      <c r="M33" s="16" t="n">
         <v>10.7801</v>
       </c>
-      <c r="N30" s="17" t="n">
+      <c r="N33" s="19" t="n">
         <v>3.9814</v>
       </c>
     </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J37" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L37" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M37" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q37" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R37" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="S37" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="T37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U37" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V37" s="1" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <v>10.870822</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>10.882502</v>
+      </c>
+      <c r="J38" s="1" t="n">
+        <v>10.886223</v>
+      </c>
+      <c r="K38" s="1" t="n">
+        <v>10.892321</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P38" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q38" s="1" t="n">
+        <v>3.70853</v>
+      </c>
+      <c r="R38" s="1" t="n">
+        <v>3.731487</v>
+      </c>
+      <c r="S38" s="1" t="n">
+        <v>3.739217</v>
+      </c>
+      <c r="T38" s="1" t="n">
+        <v>3.753091</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <v>10.746724</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>10.74607</v>
+      </c>
+      <c r="J39" s="1" t="n">
+        <v>10.754241</v>
+      </c>
+      <c r="K39" s="1" t="n">
+        <v>10.787461</v>
+      </c>
+      <c r="P39" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q39" s="1" t="n">
+        <v>3.646528</v>
+      </c>
+      <c r="R39" s="1" t="n">
+        <v>3.676749</v>
+      </c>
+      <c r="S39" s="1" t="n">
+        <v>3.696475</v>
+      </c>
+      <c r="T39" s="1" t="n">
+        <v>3.765441</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <v>10.723729</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>10.712326</v>
+      </c>
+      <c r="J40" s="1" t="n">
+        <v>10.716463</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <v>10.757103</v>
+      </c>
+      <c r="P40" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q40" s="1" t="n">
+        <v>3.645647</v>
+      </c>
+      <c r="R40" s="1" t="n">
+        <v>3.68095</v>
+      </c>
+      <c r="S40" s="1" t="n">
+        <v>3.702252</v>
+      </c>
+      <c r="T40" s="1" t="n">
+        <v>3.790243</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>10.674587</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>10.650764</v>
+      </c>
+      <c r="J41" s="1" t="n">
+        <v>10.654321</v>
+      </c>
+      <c r="P41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="1" t="n">
+        <v>3.640026</v>
+      </c>
+      <c r="R41" s="1" t="n">
+        <v>3.706047</v>
+      </c>
+      <c r="S41" s="1" t="n">
+        <v>3.744059</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G42" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <v>10.662423</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>10.634115</v>
+      </c>
+      <c r="J42" s="1" t="n">
+        <v>10.635713</v>
+      </c>
+      <c r="P42" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q42" s="1" t="n">
+        <v>3.639276</v>
+      </c>
+      <c r="R42" s="1" t="n">
+        <v>3.720625</v>
+      </c>
+      <c r="S42" s="1" t="n">
+        <v>3.767024</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G43" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>10.650457</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>10.616083</v>
+      </c>
+      <c r="J43" s="1" t="n">
+        <v>10.616554</v>
+      </c>
+      <c r="P43" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Q43" s="1" t="n">
+        <v>3.639203</v>
+      </c>
+      <c r="R43" s="1" t="n">
+        <v>3.74898</v>
+      </c>
+      <c r="S43" s="1" t="n">
+        <v>3.81797</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="M4:N4"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="Q36:V36"/>
+    <mergeCell ref="F38:F43"/>
+    <mergeCell ref="O38:O43"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
all work done on April 26th
</commit_message>
<xml_diff>
--- a/experimental_results.xlsx
+++ b/experimental_results.xlsx
@@ -5,17 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hydrangea" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Urban 2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="30">
   <si>
     <t>Urban 2</t>
   </si>
@@ -103,6 +105,9 @@
   <si>
     <t>combined rmse</t>
   </si>
+  <si>
+    <t>Hydrangea</t>
+  </si>
 </sst>
 </file>
 
@@ -111,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -144,6 +149,18 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF228B22"/>
+      <name val="lucidatypewriter"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -256,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -333,6 +350,30 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -353,7 +394,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF228B22"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -412,8 +453,8 @@
   </sheetPr>
   <dimension ref="B1:U60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q59" activeCellId="0" sqref="Q59"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2113,4 +2154,2152 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L38"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O21" activeCellId="0" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="19" width="8.61224489795918"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="21"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="19" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="J4" s="19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="K4" s="19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="L4" s="19" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="19" t="n">
+        <v>100</v>
+      </c>
+      <c r="C5" s="19" t="n">
+        <v>3.415445</v>
+      </c>
+      <c r="D5" s="19" t="n">
+        <v>3.437446</v>
+      </c>
+      <c r="E5" s="19" t="n">
+        <v>3.444015</v>
+      </c>
+      <c r="F5" s="19" t="n">
+        <v>3.455648</v>
+      </c>
+      <c r="G5" s="19" t="n">
+        <v>3.458204</v>
+      </c>
+      <c r="H5" s="19" t="n">
+        <v>3.460435</v>
+      </c>
+      <c r="I5" s="19" t="n">
+        <v>3.46071</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="23"/>
+      <c r="B6" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" s="19" t="n">
+        <v>3.198597</v>
+      </c>
+      <c r="D6" s="19" t="n">
+        <v>3.23239</v>
+      </c>
+      <c r="E6" s="19" t="n">
+        <v>3.241412</v>
+      </c>
+      <c r="F6" s="19" t="n">
+        <v>3.278638</v>
+      </c>
+      <c r="G6" s="19" t="n">
+        <v>3.302365</v>
+      </c>
+      <c r="H6" s="19" t="n">
+        <v>3.345967</v>
+      </c>
+      <c r="I6" s="19" t="n">
+        <v>3.35584</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23"/>
+      <c r="B7" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="19" t="n">
+        <v>3.154025</v>
+      </c>
+      <c r="D7" s="19" t="n">
+        <v>3.201641</v>
+      </c>
+      <c r="E7" s="19" t="n">
+        <v>3.204188</v>
+      </c>
+      <c r="F7" s="19" t="n">
+        <v>3.247206</v>
+      </c>
+      <c r="G7" s="19" t="n">
+        <v>3.275462</v>
+      </c>
+      <c r="H7" s="19" t="n">
+        <v>3.348041</v>
+      </c>
+      <c r="I7" s="19" t="n">
+        <v>3.368311</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23"/>
+      <c r="B8" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="19" t="n">
+        <v>3.112911</v>
+      </c>
+      <c r="D8" s="19" t="n">
+        <v>3.178876</v>
+      </c>
+      <c r="E8" s="19" t="n">
+        <v>3.189541</v>
+      </c>
+      <c r="F8" s="19" t="n">
+        <v>3.265608</v>
+      </c>
+      <c r="G8" s="19" t="n">
+        <v>3.304919</v>
+      </c>
+      <c r="H8" s="19" t="n">
+        <v>3.408202</v>
+      </c>
+      <c r="I8" s="19" t="n">
+        <v>3.463255</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23"/>
+      <c r="B9" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="19" t="n">
+        <v>3.107948</v>
+      </c>
+      <c r="D9" s="19" t="n">
+        <v>3.176681</v>
+      </c>
+      <c r="E9" s="19" t="n">
+        <v>3.194051</v>
+      </c>
+      <c r="F9" s="19" t="n">
+        <v>3.294498</v>
+      </c>
+      <c r="G9" s="19" t="n">
+        <v>3.343492</v>
+      </c>
+      <c r="H9" s="19" t="n">
+        <v>3.457805</v>
+      </c>
+      <c r="I9" s="19" t="n">
+        <v>3.517026</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23"/>
+      <c r="B10" s="19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="19" t="n">
+        <v>3.105033</v>
+      </c>
+      <c r="D10" s="19" t="n">
+        <v>3.177206</v>
+      </c>
+      <c r="E10" s="19" t="n">
+        <v>3.202467</v>
+      </c>
+      <c r="F10" s="19" t="n">
+        <v>3.339275</v>
+      </c>
+      <c r="G10" s="19" t="n">
+        <v>3.427288</v>
+      </c>
+      <c r="H10" s="19" t="n">
+        <v>3.597256</v>
+      </c>
+      <c r="I10" s="19" t="n">
+        <v>3.665904</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="23"/>
+      <c r="B11" s="19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C11" s="19" t="n">
+        <v>3.103676</v>
+      </c>
+      <c r="D11" s="19" t="n">
+        <v>3.177843</v>
+      </c>
+      <c r="E11" s="19" t="n">
+        <v>3.204998</v>
+      </c>
+      <c r="F11" s="19" t="n">
+        <v>3.35435</v>
+      </c>
+      <c r="G11" s="19" t="n">
+        <v>3.443211</v>
+      </c>
+      <c r="H11" s="19" t="n">
+        <v>3.645728</v>
+      </c>
+      <c r="I11" s="19" t="n">
+        <v>3.724035</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="23"/>
+      <c r="B12" s="19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C12" s="19" t="n">
+        <v>3.1014</v>
+      </c>
+      <c r="D12" s="19" t="n">
+        <v>3.178569</v>
+      </c>
+      <c r="E12" s="19" t="n">
+        <v>3.207599</v>
+      </c>
+      <c r="F12" s="19" t="n">
+        <v>3.37169</v>
+      </c>
+      <c r="G12" s="19" t="n">
+        <v>3.466834</v>
+      </c>
+      <c r="H12" s="19" t="n">
+        <v>3.713395</v>
+      </c>
+      <c r="I12" s="19" t="n">
+        <v>3.828686</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23"/>
+      <c r="B13" s="19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="C13" s="19" t="n">
+        <v>3.101121</v>
+      </c>
+      <c r="D13" s="19" t="n">
+        <v>3.178616</v>
+      </c>
+      <c r="E13" s="19" t="n">
+        <v>3.207962</v>
+      </c>
+      <c r="F13" s="19" t="n">
+        <v>3.374364</v>
+      </c>
+      <c r="G13" s="19" t="n">
+        <v>3.471136</v>
+      </c>
+      <c r="H13" s="19" t="n">
+        <v>3.728833</v>
+      </c>
+      <c r="I13" s="19" t="n">
+        <v>3.852795</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="23"/>
+      <c r="B14" s="19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C14" s="19" t="n">
+        <v>3.100828</v>
+      </c>
+      <c r="D14" s="19" t="n">
+        <v>3.178724</v>
+      </c>
+      <c r="E14" s="19" t="n">
+        <v>3.208257</v>
+      </c>
+      <c r="F14" s="19" t="n">
+        <v>3.376608</v>
+      </c>
+      <c r="G14" s="19" t="n">
+        <v>3.47489</v>
+      </c>
+      <c r="H14" s="19" t="n">
+        <v>3.743798</v>
+      </c>
+      <c r="I14" s="19" t="n">
+        <v>3.876076</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="19" t="n">
+        <v>100</v>
+      </c>
+      <c r="D17" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="F17" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H17" s="19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="J17" s="19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="K17" s="19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="L17" s="19" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="19" t="n">
+        <v>100</v>
+      </c>
+      <c r="C18" s="19" t="n">
+        <v>0.583256</v>
+      </c>
+      <c r="D18" s="19" t="n">
+        <v>0.679741</v>
+      </c>
+      <c r="E18" s="19" t="n">
+        <v>0.708444</v>
+      </c>
+      <c r="F18" s="19" t="n">
+        <v>0.754908</v>
+      </c>
+      <c r="G18" s="19" t="n">
+        <v>0.764694</v>
+      </c>
+      <c r="H18" s="19" t="n">
+        <v>0.774333</v>
+      </c>
+      <c r="I18" s="19" t="n">
+        <v>0.775754</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="23"/>
+      <c r="B19" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="C19" s="19" t="n">
+        <v>0.611377</v>
+      </c>
+      <c r="D19" s="19" t="n">
+        <v>0.812039</v>
+      </c>
+      <c r="E19" s="19" t="n">
+        <v>0.884077</v>
+      </c>
+      <c r="F19" s="19" t="n">
+        <v>1.070414</v>
+      </c>
+      <c r="G19" s="19" t="n">
+        <v>1.145946</v>
+      </c>
+      <c r="H19" s="19" t="n">
+        <v>1.263085</v>
+      </c>
+      <c r="I19" s="19" t="n">
+        <v>1.28655</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="23"/>
+      <c r="B20" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="19" t="n">
+        <v>0.626528</v>
+      </c>
+      <c r="D20" s="19" t="n">
+        <v>0.859558</v>
+      </c>
+      <c r="E20" s="19" t="n">
+        <v>0.940083</v>
+      </c>
+      <c r="F20" s="19" t="n">
+        <v>1.151033</v>
+      </c>
+      <c r="G20" s="19" t="n">
+        <v>1.247365</v>
+      </c>
+      <c r="H20" s="19" t="n">
+        <v>1.422285</v>
+      </c>
+      <c r="I20" s="19" t="n">
+        <v>1.465386</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="23"/>
+      <c r="B21" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="19" t="n">
+        <v>0.649675</v>
+      </c>
+      <c r="D21" s="19" t="n">
+        <v>0.963937</v>
+      </c>
+      <c r="E21" s="19" t="n">
+        <v>1.070121</v>
+      </c>
+      <c r="F21" s="19" t="n">
+        <v>1.316354</v>
+      </c>
+      <c r="G21" s="19" t="n">
+        <v>1.426248</v>
+      </c>
+      <c r="H21" s="19" t="n">
+        <v>1.700077</v>
+      </c>
+      <c r="I21" s="19" t="n">
+        <v>1.800771</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="23"/>
+      <c r="B22" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="19" t="n">
+        <v>0.654156</v>
+      </c>
+      <c r="D22" s="19" t="n">
+        <v>0.995888</v>
+      </c>
+      <c r="E22" s="19" t="n">
+        <v>1.116304</v>
+      </c>
+      <c r="F22" s="19" t="n">
+        <v>1.385281</v>
+      </c>
+      <c r="G22" s="19" t="n">
+        <v>1.497621</v>
+      </c>
+      <c r="H22" s="19" t="n">
+        <v>1.771059</v>
+      </c>
+      <c r="I22" s="19" t="n">
+        <v>1.887432</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="23"/>
+      <c r="B23" s="19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="19" t="n">
+        <v>0.658225</v>
+      </c>
+      <c r="D23" s="19" t="n">
+        <v>1.033501</v>
+      </c>
+      <c r="E23" s="19" t="n">
+        <v>1.179219</v>
+      </c>
+      <c r="F23" s="19" t="n">
+        <v>1.519594</v>
+      </c>
+      <c r="G23" s="19" t="n">
+        <v>1.643471</v>
+      </c>
+      <c r="H23" s="19" t="n">
+        <v>1.920279</v>
+      </c>
+      <c r="I23" s="19" t="n">
+        <v>2.033775</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="23"/>
+      <c r="B24" s="19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C24" s="19" t="n">
+        <v>0.658767</v>
+      </c>
+      <c r="D24" s="19" t="n">
+        <v>1.039513</v>
+      </c>
+      <c r="E24" s="19" t="n">
+        <v>1.190571</v>
+      </c>
+      <c r="F24" s="19" t="n">
+        <v>1.554068</v>
+      </c>
+      <c r="G24" s="19" t="n">
+        <v>1.693586</v>
+      </c>
+      <c r="H24" s="19" t="n">
+        <v>1.983927</v>
+      </c>
+      <c r="I24" s="19" t="n">
+        <v>2.103139</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="23"/>
+      <c r="B25" s="19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C25" s="19" t="n">
+        <v>0.659204</v>
+      </c>
+      <c r="D25" s="19" t="n">
+        <v>1.044622</v>
+      </c>
+      <c r="E25" s="19" t="n">
+        <v>1.200606</v>
+      </c>
+      <c r="F25" s="19" t="n">
+        <v>1.590172</v>
+      </c>
+      <c r="G25" s="19" t="n">
+        <v>1.752956</v>
+      </c>
+      <c r="H25" s="19" t="n">
+        <v>2.098956</v>
+      </c>
+      <c r="I25" s="19" t="n">
+        <v>2.21592</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="23"/>
+      <c r="B26" s="19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="C26" s="19" t="n">
+        <v>0.659259</v>
+      </c>
+      <c r="D26" s="19" t="n">
+        <v>1.045285</v>
+      </c>
+      <c r="E26" s="19" t="n">
+        <v>1.20193</v>
+      </c>
+      <c r="F26" s="19" t="n">
+        <v>1.595461</v>
+      </c>
+      <c r="G26" s="19" t="n">
+        <v>1.762476</v>
+      </c>
+      <c r="H26" s="19" t="n">
+        <v>2.123259</v>
+      </c>
+      <c r="I26" s="19" t="n">
+        <v>2.240642</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="23"/>
+      <c r="B27" s="19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C27" s="19" t="n">
+        <v>0.659303</v>
+      </c>
+      <c r="D27" s="19" t="n">
+        <v>1.045814</v>
+      </c>
+      <c r="E27" s="19" t="n">
+        <v>1.203002</v>
+      </c>
+      <c r="F27" s="19" t="n">
+        <v>1.599848</v>
+      </c>
+      <c r="G27" s="19" t="n">
+        <v>1.770591</v>
+      </c>
+      <c r="H27" s="19" t="n">
+        <v>2.14596</v>
+      </c>
+      <c r="I27" s="19" t="n">
+        <v>2.264207</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="19" t="n">
+        <f aca="false">(C5+C18)/2</f>
+        <v>1.9993505</v>
+      </c>
+      <c r="D29" s="19" t="n">
+        <f aca="false">(D5+D18)/2</f>
+        <v>2.0585935</v>
+      </c>
+      <c r="E29" s="19" t="n">
+        <f aca="false">(E5+E18)/2</f>
+        <v>2.0762295</v>
+      </c>
+      <c r="F29" s="19" t="n">
+        <f aca="false">(F5+F18)/2</f>
+        <v>2.105278</v>
+      </c>
+      <c r="G29" s="19" t="n">
+        <f aca="false">(G5+G18)/2</f>
+        <v>2.111449</v>
+      </c>
+      <c r="H29" s="19" t="n">
+        <f aca="false">(H5+H18)/2</f>
+        <v>2.117384</v>
+      </c>
+      <c r="I29" s="19" t="n">
+        <f aca="false">(I5+I18)/2</f>
+        <v>2.118232</v>
+      </c>
+      <c r="J29" s="19" t="n">
+        <f aca="false">(J5+J18)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="19" t="n">
+        <f aca="false">(K5+K18)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="19" t="n">
+        <f aca="false">(L5+L18)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="19" t="n">
+        <f aca="false">(C6+C19)/2</f>
+        <v>1.904987</v>
+      </c>
+      <c r="D30" s="19" t="n">
+        <f aca="false">(D6+D19)/2</f>
+        <v>2.0222145</v>
+      </c>
+      <c r="E30" s="19" t="n">
+        <f aca="false">(E6+E19)/2</f>
+        <v>2.0627445</v>
+      </c>
+      <c r="F30" s="19" t="n">
+        <f aca="false">(F6+F19)/2</f>
+        <v>2.174526</v>
+      </c>
+      <c r="G30" s="19" t="n">
+        <f aca="false">(G6+G19)/2</f>
+        <v>2.2241555</v>
+      </c>
+      <c r="H30" s="19" t="n">
+        <f aca="false">(H6+H19)/2</f>
+        <v>2.304526</v>
+      </c>
+      <c r="I30" s="19" t="n">
+        <f aca="false">(I6+I19)/2</f>
+        <v>2.321195</v>
+      </c>
+      <c r="J30" s="19" t="n">
+        <f aca="false">(J6+J19)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="19" t="n">
+        <f aca="false">(K6+K19)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="19" t="n">
+        <f aca="false">(L6+L19)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="19" t="n">
+        <f aca="false">(C7+C20)/2</f>
+        <v>1.8902765</v>
+      </c>
+      <c r="D31" s="19" t="n">
+        <f aca="false">(D7+D20)/2</f>
+        <v>2.0305995</v>
+      </c>
+      <c r="E31" s="19" t="n">
+        <f aca="false">(E7+E20)/2</f>
+        <v>2.0721355</v>
+      </c>
+      <c r="F31" s="19" t="n">
+        <f aca="false">(F7+F20)/2</f>
+        <v>2.1991195</v>
+      </c>
+      <c r="G31" s="19" t="n">
+        <f aca="false">(G7+G20)/2</f>
+        <v>2.2614135</v>
+      </c>
+      <c r="H31" s="19" t="n">
+        <f aca="false">(H7+H20)/2</f>
+        <v>2.385163</v>
+      </c>
+      <c r="I31" s="19" t="n">
+        <f aca="false">(I7+I20)/2</f>
+        <v>2.4168485</v>
+      </c>
+      <c r="J31" s="19" t="n">
+        <f aca="false">(J7+J20)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="19" t="n">
+        <f aca="false">(K7+K20)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="19" t="n">
+        <f aca="false">(L7+L20)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="19" t="n">
+        <f aca="false">(C8+C21)/2</f>
+        <v>1.881293</v>
+      </c>
+      <c r="D32" s="19" t="n">
+        <f aca="false">(D8+D21)/2</f>
+        <v>2.0714065</v>
+      </c>
+      <c r="E32" s="19" t="n">
+        <f aca="false">(E8+E21)/2</f>
+        <v>2.129831</v>
+      </c>
+      <c r="F32" s="19" t="n">
+        <f aca="false">(F8+F21)/2</f>
+        <v>2.290981</v>
+      </c>
+      <c r="G32" s="19" t="n">
+        <f aca="false">(G8+G21)/2</f>
+        <v>2.3655835</v>
+      </c>
+      <c r="H32" s="19" t="n">
+        <f aca="false">(H8+H21)/2</f>
+        <v>2.5541395</v>
+      </c>
+      <c r="I32" s="19" t="n">
+        <f aca="false">(I8+I21)/2</f>
+        <v>2.632013</v>
+      </c>
+      <c r="J32" s="19" t="n">
+        <f aca="false">(J8+J21)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K32" s="19" t="n">
+        <f aca="false">(K8+K21)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="19" t="n">
+        <f aca="false">(L8+L21)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="19" t="n">
+        <f aca="false">(C9+C22)/2</f>
+        <v>1.881052</v>
+      </c>
+      <c r="D33" s="19" t="n">
+        <f aca="false">(D9+D22)/2</f>
+        <v>2.0862845</v>
+      </c>
+      <c r="E33" s="19" t="n">
+        <f aca="false">(E9+E22)/2</f>
+        <v>2.1551775</v>
+      </c>
+      <c r="F33" s="19" t="n">
+        <f aca="false">(F9+F22)/2</f>
+        <v>2.3398895</v>
+      </c>
+      <c r="G33" s="19" t="n">
+        <f aca="false">(G9+G22)/2</f>
+        <v>2.4205565</v>
+      </c>
+      <c r="H33" s="19" t="n">
+        <f aca="false">(H9+H22)/2</f>
+        <v>2.614432</v>
+      </c>
+      <c r="I33" s="19" t="n">
+        <f aca="false">(I9+I22)/2</f>
+        <v>2.702229</v>
+      </c>
+      <c r="J33" s="19" t="n">
+        <f aca="false">(J9+J22)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="19" t="n">
+        <f aca="false">(K9+K22)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="19" t="n">
+        <f aca="false">(L9+L22)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="19" t="n">
+        <f aca="false">(C10+C23)/2</f>
+        <v>1.881629</v>
+      </c>
+      <c r="D34" s="19" t="n">
+        <f aca="false">(D10+D23)/2</f>
+        <v>2.1053535</v>
+      </c>
+      <c r="E34" s="19" t="n">
+        <f aca="false">(E10+E23)/2</f>
+        <v>2.190843</v>
+      </c>
+      <c r="F34" s="19" t="n">
+        <f aca="false">(F10+F23)/2</f>
+        <v>2.4294345</v>
+      </c>
+      <c r="G34" s="19" t="n">
+        <f aca="false">(G10+G23)/2</f>
+        <v>2.5353795</v>
+      </c>
+      <c r="H34" s="19" t="n">
+        <f aca="false">(H10+H23)/2</f>
+        <v>2.7587675</v>
+      </c>
+      <c r="I34" s="19" t="n">
+        <f aca="false">(I10+I23)/2</f>
+        <v>2.8498395</v>
+      </c>
+      <c r="J34" s="19" t="n">
+        <f aca="false">(J10+J23)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="19" t="n">
+        <f aca="false">(K10+K23)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L34" s="19" t="n">
+        <f aca="false">(L10+L23)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="19" t="n">
+        <f aca="false">(C11+C24)/2</f>
+        <v>1.8812215</v>
+      </c>
+      <c r="D35" s="19" t="n">
+        <f aca="false">(D11+D24)/2</f>
+        <v>2.108678</v>
+      </c>
+      <c r="E35" s="19" t="n">
+        <f aca="false">(E11+E24)/2</f>
+        <v>2.1977845</v>
+      </c>
+      <c r="F35" s="19" t="n">
+        <f aca="false">(F11+F24)/2</f>
+        <v>2.454209</v>
+      </c>
+      <c r="G35" s="19" t="n">
+        <f aca="false">(G11+G24)/2</f>
+        <v>2.5683985</v>
+      </c>
+      <c r="H35" s="19" t="n">
+        <f aca="false">(H11+H24)/2</f>
+        <v>2.8148275</v>
+      </c>
+      <c r="I35" s="19" t="n">
+        <f aca="false">(I11+I24)/2</f>
+        <v>2.913587</v>
+      </c>
+      <c r="J35" s="19" t="n">
+        <f aca="false">(J11+J24)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="19" t="n">
+        <f aca="false">(K11+K24)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="19" t="n">
+        <f aca="false">(L11+L24)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="19" t="n">
+        <f aca="false">(C12+C25)/2</f>
+        <v>1.880302</v>
+      </c>
+      <c r="D36" s="19" t="n">
+        <f aca="false">(D12+D25)/2</f>
+        <v>2.1115955</v>
+      </c>
+      <c r="E36" s="19" t="n">
+        <f aca="false">(E12+E25)/2</f>
+        <v>2.2041025</v>
+      </c>
+      <c r="F36" s="19" t="n">
+        <f aca="false">(F12+F25)/2</f>
+        <v>2.480931</v>
+      </c>
+      <c r="G36" s="19" t="n">
+        <f aca="false">(G12+G25)/2</f>
+        <v>2.609895</v>
+      </c>
+      <c r="H36" s="19" t="n">
+        <f aca="false">(H12+H25)/2</f>
+        <v>2.9061755</v>
+      </c>
+      <c r="I36" s="19" t="n">
+        <f aca="false">(I12+I25)/2</f>
+        <v>3.022303</v>
+      </c>
+      <c r="J36" s="19" t="n">
+        <f aca="false">(J12+J25)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="19" t="n">
+        <f aca="false">(K12+K25)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="19" t="n">
+        <f aca="false">(L12+L25)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="19" t="n">
+        <f aca="false">(C13+C26)/2</f>
+        <v>1.88019</v>
+      </c>
+      <c r="D37" s="19" t="n">
+        <f aca="false">(D13+D26)/2</f>
+        <v>2.1119505</v>
+      </c>
+      <c r="E37" s="19" t="n">
+        <f aca="false">(E13+E26)/2</f>
+        <v>2.204946</v>
+      </c>
+      <c r="F37" s="19" t="n">
+        <f aca="false">(F13+F26)/2</f>
+        <v>2.4849125</v>
+      </c>
+      <c r="G37" s="19" t="n">
+        <f aca="false">(G13+G26)/2</f>
+        <v>2.616806</v>
+      </c>
+      <c r="H37" s="19" t="n">
+        <f aca="false">(H13+H26)/2</f>
+        <v>2.926046</v>
+      </c>
+      <c r="I37" s="19" t="n">
+        <f aca="false">(I13+I26)/2</f>
+        <v>3.0467185</v>
+      </c>
+      <c r="J37" s="19" t="n">
+        <f aca="false">(J13+J26)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="19" t="n">
+        <f aca="false">(K13+K26)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="19" t="n">
+        <f aca="false">(L13+L26)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="19" t="n">
+        <f aca="false">(C14+C27)/2</f>
+        <v>1.8800655</v>
+      </c>
+      <c r="D38" s="19" t="n">
+        <f aca="false">(D14+D27)/2</f>
+        <v>2.112269</v>
+      </c>
+      <c r="E38" s="19" t="n">
+        <f aca="false">(E14+E27)/2</f>
+        <v>2.2056295</v>
+      </c>
+      <c r="F38" s="19" t="n">
+        <f aca="false">(F14+F27)/2</f>
+        <v>2.488228</v>
+      </c>
+      <c r="G38" s="19" t="n">
+        <f aca="false">(G14+G27)/2</f>
+        <v>2.6227405</v>
+      </c>
+      <c r="H38" s="19" t="n">
+        <f aca="false">(H14+H27)/2</f>
+        <v>2.944879</v>
+      </c>
+      <c r="I38" s="19" t="n">
+        <f aca="false">(I14+I27)/2</f>
+        <v>3.0701415</v>
+      </c>
+      <c r="J38" s="19" t="n">
+        <f aca="false">(J14+J27)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K38" s="19" t="n">
+        <f aca="false">(K14+K27)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="19" t="n">
+        <f aca="false">(L14+L27)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="C16:L16"/>
+    <mergeCell ref="A18:A27"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N41"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="8.61224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="19" width="9.90816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="8.61224489795918"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="24" t="n">
+        <v>500</v>
+      </c>
+      <c r="D4" s="24" t="n">
+        <v>200</v>
+      </c>
+      <c r="E4" s="19" t="n">
+        <v>100</v>
+      </c>
+      <c r="F4" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K4" s="19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="L4" s="19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M4" s="19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="N4" s="19" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="19" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" s="19" t="n">
+        <v>10.858039</v>
+      </c>
+      <c r="F5" s="19" t="n">
+        <v>10.878281</v>
+      </c>
+      <c r="G5" s="19" t="n">
+        <v>10.883463</v>
+      </c>
+      <c r="H5" s="19" t="n">
+        <v>10.890545</v>
+      </c>
+      <c r="I5" s="19" t="n">
+        <v>10.891921</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="23"/>
+      <c r="B6" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" s="19" t="n">
+        <v>10.703181</v>
+      </c>
+      <c r="F6" s="19" t="n">
+        <v>10.716563</v>
+      </c>
+      <c r="G6" s="19" t="n">
+        <v>10.729772</v>
+      </c>
+      <c r="H6" s="19" t="n">
+        <v>10.77354</v>
+      </c>
+      <c r="I6" s="19" t="n">
+        <v>10.793144</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23"/>
+      <c r="B7" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" s="19" t="n">
+        <v>10.672203</v>
+      </c>
+      <c r="F7" s="19" t="n">
+        <v>10.671697</v>
+      </c>
+      <c r="G7" s="19" t="n">
+        <v>10.682221</v>
+      </c>
+      <c r="H7" s="19" t="n">
+        <v>10.731799</v>
+      </c>
+      <c r="I7" s="19" t="n">
+        <v>10.76089</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23"/>
+      <c r="B8" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19" t="n">
+        <v>10.631809</v>
+      </c>
+      <c r="F8" s="19" t="n">
+        <v>10.600763</v>
+      </c>
+      <c r="G8" s="19" t="n">
+        <v>10.6042</v>
+      </c>
+      <c r="H8" s="19" t="n">
+        <v>10.660204</v>
+      </c>
+      <c r="I8" s="19" t="n">
+        <v>10.702291</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23"/>
+      <c r="B9" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="19" t="n">
+        <v>10.617017</v>
+      </c>
+      <c r="F9" s="19" t="n">
+        <v>10.584843</v>
+      </c>
+      <c r="G9" s="19" t="n">
+        <v>10.585458</v>
+      </c>
+      <c r="H9" s="19" t="n">
+        <v>10.644186</v>
+      </c>
+      <c r="I9" s="19" t="n">
+        <v>10.69791</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23"/>
+      <c r="B10" s="19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="19" t="n">
+        <v>10.600737</v>
+      </c>
+      <c r="F10" s="19" t="n">
+        <v>10.570302</v>
+      </c>
+      <c r="G10" s="19" t="n">
+        <v>10.570126</v>
+      </c>
+      <c r="H10" s="19" t="n">
+        <v>10.639805</v>
+      </c>
+      <c r="I10" s="19" t="n">
+        <v>10.708136</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="23"/>
+      <c r="B11" s="19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E11" s="19" t="n">
+        <v>10.59829</v>
+      </c>
+      <c r="F11" s="19" t="n">
+        <v>10.568611</v>
+      </c>
+      <c r="G11" s="19" t="n">
+        <v>10.569282</v>
+      </c>
+      <c r="H11" s="19" t="n">
+        <v>10.646752</v>
+      </c>
+      <c r="I11" s="19" t="n">
+        <v>10.721829</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="23"/>
+      <c r="B12" s="19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E12" s="19" t="n">
+        <v>10.596239</v>
+      </c>
+      <c r="F12" s="19" t="n">
+        <v>10.56745</v>
+      </c>
+      <c r="G12" s="19" t="n">
+        <v>10.569298</v>
+      </c>
+      <c r="H12" s="19" t="n">
+        <v>10.659821</v>
+      </c>
+      <c r="I12" s="19" t="n">
+        <v>10.747935</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23"/>
+      <c r="B13" s="19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E13" s="19" t="n">
+        <v>10.595985</v>
+      </c>
+      <c r="F13" s="19" t="n">
+        <v>10.566996</v>
+      </c>
+      <c r="G13" s="19" t="n">
+        <v>10.569361</v>
+      </c>
+      <c r="H13" s="19" t="n">
+        <v>10.662528</v>
+      </c>
+      <c r="I13" s="19" t="n">
+        <v>10.753797</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="23"/>
+      <c r="B14" s="19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C14" s="19" t="n">
+        <v>10.6666</v>
+      </c>
+      <c r="D14" s="19" t="n">
+        <v>10.6299</v>
+      </c>
+      <c r="E14" s="19" t="n">
+        <v>10.595733</v>
+      </c>
+      <c r="F14" s="19" t="n">
+        <v>10.566509</v>
+      </c>
+      <c r="G14" s="19" t="n">
+        <v>10.569437</v>
+      </c>
+      <c r="H14" s="19" t="n">
+        <v>10.664962</v>
+      </c>
+      <c r="I14" s="19" t="n">
+        <v>10.759246</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="19" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C15" s="19" t="n">
+        <v>10.6666</v>
+      </c>
+      <c r="D15" s="19" t="n">
+        <v>10.6298</v>
+      </c>
+      <c r="E15" s="19" t="n">
+        <v>10.5957</v>
+      </c>
+      <c r="F15" s="19" t="n">
+        <v>10.5664</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E18" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="19" t="n">
+        <v>100</v>
+      </c>
+      <c r="F19" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="G19" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="H19" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J19" s="19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K19" s="19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="L19" s="19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M19" s="19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="N19" s="19" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="19" t="n">
+        <v>100</v>
+      </c>
+      <c r="E20" s="19" t="n">
+        <v>3.702477</v>
+      </c>
+      <c r="F20" s="19" t="n">
+        <v>3.730936</v>
+      </c>
+      <c r="G20" s="19" t="n">
+        <v>3.739573</v>
+      </c>
+      <c r="H20" s="19" t="n">
+        <v>3.753073</v>
+      </c>
+      <c r="I20" s="19" t="n">
+        <v>3.755925</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="23"/>
+      <c r="B21" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" s="19" t="n">
+        <v>3.630851</v>
+      </c>
+      <c r="F21" s="19" t="n">
+        <v>3.664091</v>
+      </c>
+      <c r="G21" s="19" t="n">
+        <v>3.685672</v>
+      </c>
+      <c r="H21" s="19" t="n">
+        <v>3.760616</v>
+      </c>
+      <c r="I21" s="19" t="n">
+        <v>3.795508</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="23"/>
+      <c r="B22" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="E22" s="19" t="n">
+        <v>3.627814</v>
+      </c>
+      <c r="F22" s="19" t="n">
+        <v>3.664015</v>
+      </c>
+      <c r="G22" s="19" t="n">
+        <v>3.687577</v>
+      </c>
+      <c r="H22" s="19" t="n">
+        <v>3.779522</v>
+      </c>
+      <c r="I22" s="19" t="n">
+        <v>3.830986</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="23"/>
+      <c r="B23" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="19" t="n">
+        <v>3.630633</v>
+      </c>
+      <c r="F23" s="19" t="n">
+        <v>3.690426</v>
+      </c>
+      <c r="G23" s="19" t="n">
+        <v>3.727402</v>
+      </c>
+      <c r="H23" s="19" t="n">
+        <v>3.867111</v>
+      </c>
+      <c r="I23" s="19" t="n">
+        <v>3.948255</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="23"/>
+      <c r="B24" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="19" t="n">
+        <v>3.628084</v>
+      </c>
+      <c r="F24" s="19" t="n">
+        <v>3.707542</v>
+      </c>
+      <c r="G24" s="19" t="n">
+        <v>3.753202</v>
+      </c>
+      <c r="H24" s="19" t="n">
+        <v>3.919252</v>
+      </c>
+      <c r="I24" s="19" t="n">
+        <v>4.014783</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="23"/>
+      <c r="B25" s="19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E25" s="19" t="n">
+        <v>3.625561</v>
+      </c>
+      <c r="F25" s="19" t="n">
+        <v>3.740521</v>
+      </c>
+      <c r="G25" s="19" t="n">
+        <v>3.810661</v>
+      </c>
+      <c r="H25" s="19" t="n">
+        <v>4.053919</v>
+      </c>
+      <c r="I25" s="19" t="n">
+        <v>4.183844</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="23"/>
+      <c r="B26" s="19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E26" s="19" t="n">
+        <v>3.625245</v>
+      </c>
+      <c r="F26" s="19" t="n">
+        <v>3.748257</v>
+      </c>
+      <c r="G26" s="19" t="n">
+        <v>3.826394</v>
+      </c>
+      <c r="H26" s="19" t="n">
+        <v>4.104461</v>
+      </c>
+      <c r="I26" s="19" t="n">
+        <v>4.253122</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="23"/>
+      <c r="B27" s="19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E27" s="19" t="n">
+        <v>3.624995</v>
+      </c>
+      <c r="F27" s="19" t="n">
+        <v>3.755755</v>
+      </c>
+      <c r="G27" s="19" t="n">
+        <v>3.842816</v>
+      </c>
+      <c r="H27" s="19" t="n">
+        <v>4.172127</v>
+      </c>
+      <c r="I27" s="19" t="n">
+        <v>4.35868</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="23"/>
+      <c r="B28" s="19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E28" s="19" t="n">
+        <v>3.624969</v>
+      </c>
+      <c r="F28" s="24" t="n">
+        <v>3.756762</v>
+      </c>
+      <c r="G28" s="19" t="n">
+        <v>3.845203</v>
+      </c>
+      <c r="H28" s="19" t="n">
+        <v>4.183768</v>
+      </c>
+      <c r="I28" s="19" t="n">
+        <v>4.378831</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="23"/>
+      <c r="B29" s="19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C29" s="19" t="n">
+        <v>3.6221</v>
+      </c>
+      <c r="D29" s="19" t="n">
+        <v>3.6228</v>
+      </c>
+      <c r="E29" s="19" t="n">
+        <v>3.624922</v>
+      </c>
+      <c r="F29" s="19" t="n">
+        <v>3.75758</v>
+      </c>
+      <c r="G29" s="19" t="n">
+        <v>3.847174</v>
+      </c>
+      <c r="H29" s="19" t="n">
+        <v>4.193842</v>
+      </c>
+      <c r="I29" s="19" t="n">
+        <v>4.396858</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="19" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C30" s="19" t="n">
+        <v>3.6221</v>
+      </c>
+      <c r="D30" s="19" t="n">
+        <v>3.6227</v>
+      </c>
+      <c r="E30" s="19" t="n">
+        <v>3.6249</v>
+      </c>
+      <c r="F30" s="19" t="n">
+        <v>3.7578</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="19" t="n">
+        <f aca="false">(E5+E20)/2</f>
+        <v>7.280258</v>
+      </c>
+      <c r="F32" s="19" t="n">
+        <f aca="false">(F5+F20)/2</f>
+        <v>7.3046085</v>
+      </c>
+      <c r="G32" s="19" t="n">
+        <f aca="false">(G5+G20)/2</f>
+        <v>7.311518</v>
+      </c>
+      <c r="H32" s="19" t="n">
+        <f aca="false">(H5+H20)/2</f>
+        <v>7.321809</v>
+      </c>
+      <c r="I32" s="19" t="n">
+        <f aca="false">(I5+I20)/2</f>
+        <v>7.323923</v>
+      </c>
+      <c r="J32" s="19" t="n">
+        <f aca="false">(J5+J20)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K32" s="19" t="n">
+        <f aca="false">(K5+K20)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="19" t="n">
+        <f aca="false">(L5+L20)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="19" t="n">
+        <f aca="false">(M5+M20)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="19" t="n">
+        <f aca="false">(N5+N20)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="19" t="n">
+        <f aca="false">(E6+E21)/2</f>
+        <v>7.167016</v>
+      </c>
+      <c r="F33" s="19" t="n">
+        <f aca="false">(F6+F21)/2</f>
+        <v>7.190327</v>
+      </c>
+      <c r="G33" s="19" t="n">
+        <f aca="false">(G6+G21)/2</f>
+        <v>7.207722</v>
+      </c>
+      <c r="H33" s="19" t="n">
+        <f aca="false">(H6+H21)/2</f>
+        <v>7.267078</v>
+      </c>
+      <c r="I33" s="19" t="n">
+        <f aca="false">(I6+I21)/2</f>
+        <v>7.294326</v>
+      </c>
+      <c r="J33" s="19" t="n">
+        <f aca="false">(J6+J21)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="19" t="n">
+        <f aca="false">(K6+K21)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="19" t="n">
+        <f aca="false">(L6+L21)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="19" t="n">
+        <f aca="false">(M6+M21)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="19" t="n">
+        <f aca="false">(N6+N21)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="19" t="n">
+        <f aca="false">(E7+E22)/2</f>
+        <v>7.1500085</v>
+      </c>
+      <c r="F34" s="19" t="n">
+        <f aca="false">(F7+F22)/2</f>
+        <v>7.167856</v>
+      </c>
+      <c r="G34" s="19" t="n">
+        <f aca="false">(G7+G22)/2</f>
+        <v>7.184899</v>
+      </c>
+      <c r="H34" s="19" t="n">
+        <f aca="false">(H7+H22)/2</f>
+        <v>7.2556605</v>
+      </c>
+      <c r="I34" s="19" t="n">
+        <f aca="false">(I7+I22)/2</f>
+        <v>7.295938</v>
+      </c>
+      <c r="J34" s="19" t="n">
+        <f aca="false">(J7+J22)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="19" t="n">
+        <f aca="false">(K7+K22)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L34" s="19" t="n">
+        <f aca="false">(L7+L22)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="19" t="n">
+        <f aca="false">(M7+M22)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="19" t="n">
+        <f aca="false">(N7+N22)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="19" t="n">
+        <f aca="false">(E8+E23)/2</f>
+        <v>7.131221</v>
+      </c>
+      <c r="F35" s="19" t="n">
+        <f aca="false">(F8+F23)/2</f>
+        <v>7.1455945</v>
+      </c>
+      <c r="G35" s="19" t="n">
+        <f aca="false">(G8+G23)/2</f>
+        <v>7.165801</v>
+      </c>
+      <c r="H35" s="19" t="n">
+        <f aca="false">(H8+H23)/2</f>
+        <v>7.2636575</v>
+      </c>
+      <c r="I35" s="19" t="n">
+        <f aca="false">(I8+I23)/2</f>
+        <v>7.325273</v>
+      </c>
+      <c r="J35" s="19" t="n">
+        <f aca="false">(J8+J23)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="19" t="n">
+        <f aca="false">(K8+K23)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="19" t="n">
+        <f aca="false">(L8+L23)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="19" t="n">
+        <f aca="false">(M8+M23)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="19" t="n">
+        <f aca="false">(N8+N23)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="19" t="n">
+        <f aca="false">(E9+E24)/2</f>
+        <v>7.1225505</v>
+      </c>
+      <c r="F36" s="19" t="n">
+        <f aca="false">(F9+F24)/2</f>
+        <v>7.1461925</v>
+      </c>
+      <c r="G36" s="19" t="n">
+        <f aca="false">(G9+G24)/2</f>
+        <v>7.16933</v>
+      </c>
+      <c r="H36" s="19" t="n">
+        <f aca="false">(H9+H24)/2</f>
+        <v>7.281719</v>
+      </c>
+      <c r="I36" s="19" t="n">
+        <f aca="false">(I9+I24)/2</f>
+        <v>7.3563465</v>
+      </c>
+      <c r="J36" s="19" t="n">
+        <f aca="false">(J9+J24)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="19" t="n">
+        <f aca="false">(K9+K24)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="19" t="n">
+        <f aca="false">(L9+L24)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="19" t="n">
+        <f aca="false">(M9+M24)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="19" t="n">
+        <f aca="false">(N9+N24)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="19" t="n">
+        <f aca="false">(E10+E25)/2</f>
+        <v>7.113149</v>
+      </c>
+      <c r="F37" s="19" t="n">
+        <f aca="false">(F10+F25)/2</f>
+        <v>7.1554115</v>
+      </c>
+      <c r="G37" s="19" t="n">
+        <f aca="false">(G10+G25)/2</f>
+        <v>7.1903935</v>
+      </c>
+      <c r="H37" s="19" t="n">
+        <f aca="false">(H10+H25)/2</f>
+        <v>7.346862</v>
+      </c>
+      <c r="I37" s="19" t="n">
+        <f aca="false">(I10+I25)/2</f>
+        <v>7.44599</v>
+      </c>
+      <c r="J37" s="19" t="n">
+        <f aca="false">(J10+J25)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="19" t="n">
+        <f aca="false">(K10+K25)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="19" t="n">
+        <f aca="false">(L10+L25)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="19" t="n">
+        <f aca="false">(M10+M25)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="19" t="n">
+        <f aca="false">(N10+N25)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="19" t="n">
+        <f aca="false">(E11+E26)/2</f>
+        <v>7.1117675</v>
+      </c>
+      <c r="F38" s="19" t="n">
+        <f aca="false">(F11+F26)/2</f>
+        <v>7.158434</v>
+      </c>
+      <c r="G38" s="19" t="n">
+        <f aca="false">(G11+G26)/2</f>
+        <v>7.197838</v>
+      </c>
+      <c r="H38" s="19" t="n">
+        <f aca="false">(H11+H26)/2</f>
+        <v>7.3756065</v>
+      </c>
+      <c r="I38" s="19" t="n">
+        <f aca="false">(I11+I26)/2</f>
+        <v>7.4874755</v>
+      </c>
+      <c r="J38" s="19" t="n">
+        <f aca="false">(J11+J26)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K38" s="19" t="n">
+        <f aca="false">(K11+K26)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="19" t="n">
+        <f aca="false">(L11+L26)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="19" t="n">
+        <f aca="false">(M11+M26)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="19" t="n">
+        <f aca="false">(N11+N26)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="19" t="n">
+        <f aca="false">(E12+E27)/2</f>
+        <v>7.110617</v>
+      </c>
+      <c r="F39" s="19" t="n">
+        <f aca="false">(F12+F27)/2</f>
+        <v>7.1616025</v>
+      </c>
+      <c r="G39" s="19" t="n">
+        <f aca="false">(G12+G27)/2</f>
+        <v>7.206057</v>
+      </c>
+      <c r="H39" s="19" t="n">
+        <f aca="false">(H12+H27)/2</f>
+        <v>7.415974</v>
+      </c>
+      <c r="I39" s="19" t="n">
+        <f aca="false">(I12+I27)/2</f>
+        <v>7.5533075</v>
+      </c>
+      <c r="J39" s="19" t="n">
+        <f aca="false">(J12+J27)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K39" s="19" t="n">
+        <f aca="false">(K12+K27)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="19" t="n">
+        <f aca="false">(L12+L27)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="19" t="n">
+        <f aca="false">(M12+M27)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="19" t="n">
+        <f aca="false">(N12+N27)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="19" t="n">
+        <f aca="false">(E13+E28)/2</f>
+        <v>7.110477</v>
+      </c>
+      <c r="F40" s="19" t="n">
+        <f aca="false">(F13+F28)/2</f>
+        <v>7.161879</v>
+      </c>
+      <c r="G40" s="19" t="n">
+        <f aca="false">(G13+G28)/2</f>
+        <v>7.207282</v>
+      </c>
+      <c r="H40" s="19" t="n">
+        <f aca="false">(H13+H28)/2</f>
+        <v>7.423148</v>
+      </c>
+      <c r="I40" s="19" t="n">
+        <f aca="false">(I13+I28)/2</f>
+        <v>7.566314</v>
+      </c>
+      <c r="J40" s="19" t="n">
+        <f aca="false">(J13+J28)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K40" s="19" t="n">
+        <f aca="false">(K13+K28)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L40" s="19" t="n">
+        <f aca="false">(L13+L28)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="19" t="n">
+        <f aca="false">(M13+M28)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="19" t="n">
+        <f aca="false">(N13+N28)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="19" t="n">
+        <f aca="false">(E14+E29)/2</f>
+        <v>7.1103275</v>
+      </c>
+      <c r="F41" s="19" t="n">
+        <f aca="false">(F14+F29)/2</f>
+        <v>7.1620445</v>
+      </c>
+      <c r="G41" s="19" t="n">
+        <f aca="false">(G14+G29)/2</f>
+        <v>7.2083055</v>
+      </c>
+      <c r="H41" s="19" t="n">
+        <f aca="false">(H14+H29)/2</f>
+        <v>7.429402</v>
+      </c>
+      <c r="I41" s="19" t="n">
+        <f aca="false">(I14+I29)/2</f>
+        <v>7.578052</v>
+      </c>
+      <c r="J41" s="19" t="n">
+        <f aca="false">(J14+J29)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K41" s="19" t="n">
+        <f aca="false">(K14+K29)/2</f>
+        <v>0</v>
+      </c>
+      <c r="L41" s="19" t="n">
+        <f aca="false">(L14+L29)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="19" t="n">
+        <f aca="false">(M14+M29)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N41" s="19" t="n">
+        <f aca="false">(N14+N29)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="E18:N18"/>
+    <mergeCell ref="A20:A29"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>